<commit_message>
merged UX-UI and File_Handler for master Run well. not test yet not recovered file yet
</commit_message>
<xml_diff>
--- a/sample/data2.xlsx
+++ b/sample/data2.xlsx
@@ -10,17 +10,17 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="vule" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
-    <t>le tran anh vu</t>
+    <t>Tran Thi Ut</t>
   </si>
   <si>
-    <t>pham thi thu trang</t>
+    <t>le tran anh vu</t>
   </si>
   <si>
     <t>s</t>
@@ -31,10 +31,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -337,17 +345,39 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1"/>
+    <row r="1" spans="1:3"/>
+    <row r="2" spans="1:3"/>
+    <row r="3" spans="1:3"/>
+    <row r="4" spans="1:3"/>
+    <row r="5" spans="1:3"/>
+    <row r="6" spans="1:3"/>
+    <row r="7" spans="1:3"/>
+    <row r="8" spans="1:3"/>
+    <row r="9" spans="1:3"/>
+    <row r="10" spans="1:3"/>
+    <row r="11" spans="1:3"/>
+    <row r="12" spans="1:3">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3"/>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -360,7 +390,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+      <selection activeCell="M9" sqref="M9:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -369,18 +399,22 @@
     <row r="2" spans="1:27"/>
     <row r="3" spans="1:27">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:27"/>
     <row r="5" spans="1:27">
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27"/>
     <row r="7" spans="1:27"/>
-    <row r="8" spans="1:27"/>
+    <row r="8" spans="1:27">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:27"/>
     <row r="10" spans="1:27"/>
     <row r="11" spans="1:27"/>

</xml_diff>

<commit_message>
bundle file. extract to exe/
</commit_message>
<xml_diff>
--- a/sample/data2.xlsx
+++ b/sample/data2.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>Tran Thi Ut</t>
+    <t>Le Tran Anh Vu</t>
   </si>
   <si>
     <t>le tran anh vu</t>
+  </si>
+  <si>
+    <t>Tran Thi Ut</t>
   </si>
   <si>
     <t>s</t>
@@ -434,10 +437,10 @@
     <row r="25" spans="1:27"/>
     <row r="26" spans="1:27">
       <c r="D26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>